<commit_message>
Base <-> Tgt mec File 비교단 적당하게 수정
</commit_message>
<xml_diff>
--- a/nGen_New_MecRT/nGen_New_MecRT/CheckerData.xlsx
+++ b/nGen_New_MecRT/nGen_New_MecRT/CheckerData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>GRID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -83,6 +83,10 @@
   </si>
   <si>
     <t>데이터 개수가 고정인 데이터만 데이터 고려 가능.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPC1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -166,11 +170,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -477,7 +481,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
+      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -742,6 +746,20 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6" spans="1:47" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+    </row>
     <row r="8" spans="1:47" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1</v>
@@ -753,67 +771,67 @@
       </c>
     </row>
     <row r="11" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
       <c r="D11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
       <c r="D12" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4" t="s">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
       <c r="D14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
       <c r="D15" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:47" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
       <c r="D16" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
       <c r="D17" t="s">
         <v>10</v>
       </c>

</xml_diff>